<commit_message>
fixed user view auth
</commit_message>
<xml_diff>
--- a/doc/sprint4_burndown.xlsx
+++ b/doc/sprint4_burndown.xlsx
@@ -167,7 +167,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -193,19 +193,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -315,7 +303,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -341,19 +329,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -463,7 +439,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -473,11 +449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="602682704"/>
-        <c:axId val="637932688"/>
+        <c:axId val="-1107556640"/>
+        <c:axId val="-1080877744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="602682704"/>
+        <c:axId val="-1107556640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42669.0"/>
@@ -592,14 +568,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="637932688"/>
+        <c:crossAx val="-1080877744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
         <c:minorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="637932688"/>
+        <c:axId val="-1080877744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="602682704"/>
+        <c:crossAx val="-1107556640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1655,7 +1631,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>